<commit_message>
exam code appended into form data
</commit_message>
<xml_diff>
--- a/ExamPortal/backend/upload/bhutan.xlsx
+++ b/ExamPortal/backend/upload/bhutan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashish.chopra\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5A389DDA-8810-4258-BCF3-D3F0C6AF1ADF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{980AB7FA-36CF-41FD-9AED-5B566DF41CAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{C5F203CF-F3BD-4073-B241-D27D6AA751EF}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="21" uniqueCount="18">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="28" uniqueCount="24">
   <si>
     <t>Bhutan</t>
   </si>
@@ -82,16 +82,42 @@
   </si>
   <si>
     <t>option4</t>
+  </si>
+  <si>
+    <t>computer was invented by?</t>
+  </si>
+  <si>
+    <t>chopra</t>
+  </si>
+  <si>
+    <t>rawat</t>
+  </si>
+  <si>
+    <t>birendra</t>
+  </si>
+  <si>
+    <t>chandan</t>
+  </si>
+  <si>
+    <t>www.chopra.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,14 +140,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -434,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E608057-4077-4E87-A5E5-F07480B12DDB}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,8 +552,37 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{DA4252DC-5F0E-4FE9-A51C-561C0C5CC64A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>